<commit_message>
completed caricoos closes #23
</commit_message>
<xml_diff>
--- a/2021/data/processed/CARICOOS.xlsx
+++ b/2021/data/processed/CARICOOS.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathew.Biddle\Documents\GitProjects\ioos-asset-inventory\2021\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EBF707-1B62-4F81-A432-07A9E4E698D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58908B1B-1B9E-412E-9CF9-3E23D358E0A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18228" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CARICOOS Asset Inventory" sheetId="1" r:id="rId1"/>
-    <sheet name="IOOS_removed" sheetId="2" r:id="rId2"/>
+    <sheet name="IOOS Removed" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -1099,10 +1099,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S992"/>
+  <dimension ref="A1:S986"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1406,88 +1406,89 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="135">
-      <c r="A6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="4">
-        <v>41051</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4">
-        <v>18.476099999999999</v>
-      </c>
-      <c r="F6" s="4">
-        <v>-65.156800000000004</v>
-      </c>
-      <c r="G6" s="4" t="s">
+    <row r="6" spans="1:19" ht="51" customHeight="1">
+      <c r="A6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="9">
+        <f>57.22/60 +17</f>
+        <v>17.953666666666667</v>
+      </c>
+      <c r="F6" s="9">
+        <v>-66.051199999999994</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="4" t="s">
+      <c r="H6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R6" s="4" t="s">
+      <c r="O6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="S6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="135">
+      <c r="S6" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="51" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="4">
-        <v>41051</v>
+        <v>74</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="4">
-        <v>18.257400000000001</v>
+        <v>18.366700000000002</v>
       </c>
       <c r="F7" s="4">
-        <v>-65.004000000000005</v>
+        <v>-67.251400000000004</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>42</v>
+        <v>77</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>15</v>
@@ -1496,110 +1497,107 @@
         <v>16</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="Q7" s="4"/>
       <c r="R7" s="4" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="51" customHeight="1">
-      <c r="A8" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="9">
-        <f>57.22/60 +17</f>
-        <v>17.953666666666667</v>
-      </c>
-      <c r="F8" s="9">
-        <v>-66.051199999999994</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="9" t="s">
+      <c r="A8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4">
+        <v>17.964400000000001</v>
+      </c>
+      <c r="F8" s="4">
+        <v>-67.044200000000004</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" s="9" t="s">
+      <c r="J8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="S8" s="9" t="s">
-        <v>69</v>
+      <c r="K8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="51" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="4">
-        <v>18.366700000000002</v>
+        <v>17.964400000000001</v>
       </c>
       <c r="F9" s="4">
-        <v>-67.251400000000004</v>
+        <v>-66.617699999999999</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>14</v>
@@ -1620,7 +1618,7 @@
         <v>15</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>82</v>
@@ -1635,35 +1633,35 @@
     </row>
     <row r="10" spans="1:19" ht="51" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="4">
-        <v>17.9694</v>
+        <v>17.933499999999999</v>
       </c>
       <c r="F10" s="4">
-        <v>-67.044200000000004</v>
+        <v>-67.191999999999993</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>79</v>
@@ -1675,14 +1673,12 @@
         <v>15</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>91</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="Q10" s="4"/>
       <c r="R10" s="4" t="s">
         <v>83</v>
       </c>
@@ -1690,28 +1686,28 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="51" customHeight="1">
+    <row r="11" spans="1:19" ht="30" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="4">
-        <v>17.964400000000001</v>
+        <v>18.347000000000001</v>
       </c>
       <c r="F11" s="4">
-        <v>-67.044200000000004</v>
+        <v>-67.261300000000006</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>14</v>
@@ -1735,11 +1731,9 @@
         <v>94</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>96</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="Q11" s="4"/>
       <c r="R11" s="4" t="s">
         <v>83</v>
       </c>
@@ -1749,50 +1743,50 @@
     </row>
     <row r="12" spans="1:19" ht="51" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4">
-        <v>17.964400000000001</v>
-      </c>
-      <c r="F12" s="4">
-        <v>-66.617699999999999</v>
+        <v>110</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14">
+        <v>18.432950000000002</v>
+      </c>
+      <c r="F12" s="14">
+        <v>-67.156630000000007</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="5" t="s">
-        <v>94</v>
+      <c r="O12" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="Q12" s="4"/>
       <c r="R12" s="4" t="s">
@@ -1804,50 +1798,50 @@
     </row>
     <row r="13" spans="1:19" ht="51" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4">
-        <v>17.933499999999999</v>
-      </c>
-      <c r="F13" s="4">
-        <v>-67.191999999999993</v>
+        <v>119</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14">
+        <v>18.34291</v>
+      </c>
+      <c r="F13" s="14">
+        <v>-64.817300000000003</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O13" s="5" t="s">
-        <v>94</v>
+      <c r="O13" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="Q13" s="4"/>
       <c r="R13" s="4" t="s">
@@ -1857,52 +1851,52 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="30" customHeight="1">
+    <row r="14" spans="1:19" ht="51" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4">
-        <v>18.347000000000001</v>
-      </c>
-      <c r="F14" s="4">
-        <v>-67.261300000000006</v>
+        <v>122</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14">
+        <v>18.278230000000001</v>
+      </c>
+      <c r="F14" s="14">
+        <v>-64.892600000000002</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O14" s="5" t="s">
-        <v>94</v>
+      <c r="O14" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="Q14" s="4"/>
       <c r="R14" s="4" t="s">
@@ -1914,26 +1908,26 @@
     </row>
     <row r="15" spans="1:19" ht="51" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="14">
-        <v>18.432950000000002</v>
+        <v>18.09995</v>
       </c>
       <c r="F15" s="14">
-        <v>-67.156630000000007</v>
+        <v>-67.188869999999994</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>14</v>
@@ -1967,37 +1961,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="51" customHeight="1">
+    <row r="16" spans="1:19" ht="30" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="4">
-        <v>18.330300000000001</v>
-      </c>
-      <c r="F16" s="4">
-        <v>-64.926400000000001</v>
+      <c r="E16" s="14">
+        <v>17.677710000000001</v>
+      </c>
+      <c r="F16" s="14">
+        <v>-64.899889999999999</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>111</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>15</v>
@@ -2024,26 +2018,26 @@
     </row>
     <row r="17" spans="1:19" ht="51" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="14">
-        <v>18.34291</v>
+        <v>18.313700000000001</v>
       </c>
       <c r="F17" s="14">
-        <v>-64.817300000000003</v>
+        <v>-65.227419999999995</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>14</v>
@@ -2079,20 +2073,20 @@
     </row>
     <row r="18" spans="1:19" ht="51" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="14">
-        <v>18.278230000000001</v>
+        <v>18.256229999999999</v>
       </c>
       <c r="F18" s="14">
-        <v>-64.892600000000002</v>
+        <v>-65.991669999999999</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>77</v>
@@ -2134,26 +2128,26 @@
     </row>
     <row r="19" spans="1:19" ht="51" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="14">
-        <v>18.09995</v>
+        <v>18.455120000000001</v>
       </c>
       <c r="F19" s="14">
-        <v>-67.188869999999994</v>
+        <v>-66.128460000000004</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>14</v>
@@ -2187,22 +2181,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="30" customHeight="1">
+    <row r="20" spans="1:19" ht="51" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="14">
-        <v>17.677710000000001</v>
+        <v>17.92859</v>
       </c>
       <c r="F20" s="14">
-        <v>-64.899889999999999</v>
+        <v>-66.159700000000001</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>77</v>
@@ -2244,26 +2238,26 @@
     </row>
     <row r="21" spans="1:19" ht="51" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="14">
-        <v>18.313700000000001</v>
+        <v>18.289380000000001</v>
       </c>
       <c r="F21" s="14">
-        <v>-65.227419999999995</v>
+        <v>-65.632000000000005</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>14</v>
@@ -2299,26 +2293,26 @@
     </row>
     <row r="22" spans="1:19" ht="51" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="14">
-        <v>18.256229999999999</v>
+        <v>18.32817</v>
       </c>
       <c r="F22" s="14">
-        <v>-65.991669999999999</v>
+        <v>-64.926609999999997</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>14</v>
@@ -2354,20 +2348,20 @@
     </row>
     <row r="23" spans="1:19" ht="51" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="14">
-        <v>18.455120000000001</v>
+        <v>18.05245</v>
       </c>
       <c r="F23" s="14">
-        <v>-66.128460000000004</v>
+        <v>-65.828090000000003</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>77</v>
@@ -2408,340 +2402,132 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="51" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14">
-        <v>17.92859</v>
-      </c>
-      <c r="F24" s="14">
-        <v>-66.159700000000001</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O24" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="P24" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="S24" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" ht="51" customHeight="1">
-      <c r="A25" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14">
-        <v>18.289380000000001</v>
-      </c>
-      <c r="F25" s="14">
-        <v>-65.632000000000005</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O25" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="P25" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="S25" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" ht="51" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="14">
-        <v>18.32817</v>
-      </c>
-      <c r="F26" s="14">
-        <v>-64.926609999999997</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O26" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="S26" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" ht="51" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14">
-        <v>18.33737</v>
-      </c>
-      <c r="F27" s="14">
-        <v>-65.082999999999998</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M27" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O27" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="P27" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q27" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="R27" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="S27" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" ht="51" customHeight="1">
-      <c r="A28" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="14">
-        <v>18.355370000000001</v>
-      </c>
-      <c r="F28" s="14">
-        <v>-64.966930000000005</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="P28" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q28" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="R28" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="S28" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" ht="51" customHeight="1">
-      <c r="A29" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14">
-        <v>18.05245</v>
-      </c>
-      <c r="F29" s="14">
-        <v>-65.828090000000003</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O29" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="P29" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="S29" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="51" customHeight="1">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="1:19" ht="30" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2783,7 +2569,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" ht="51" customHeight="1">
+    <row r="32" spans="1:19" ht="30" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2825,7 +2611,7 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" ht="51" customHeight="1">
+    <row r="34" spans="1:19" ht="30" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2867,7 +2653,7 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="1:19" ht="30" customHeight="1">
+    <row r="36" spans="1:19" ht="51" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2909,7 +2695,7 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="1:19" ht="30" customHeight="1">
+    <row r="38" spans="1:19" ht="51" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2951,7 +2737,7 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="1:19" ht="30" customHeight="1">
+    <row r="40" spans="1:19" ht="51" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3393,27 +3179,27 @@
       <c r="S60" s="1"/>
     </row>
     <row r="61" spans="1:19" ht="51" customHeight="1">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-      <c r="S61" s="1"/>
-    </row>
-    <row r="62" spans="1:19" ht="51" customHeight="1">
+      <c r="A61" s="15"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="15"/>
+      <c r="S61" s="15"/>
+    </row>
+    <row r="62" spans="1:19" ht="30" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3428,7 +3214,7 @@
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
+      <c r="O62" s="16"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
@@ -3444,8 +3230,8 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
+      <c r="J63" s="16"/>
+      <c r="K63" s="16"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
@@ -3465,8 +3251,8 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
@@ -3486,8 +3272,8 @@
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
@@ -3507,8 +3293,8 @@
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
@@ -3519,27 +3305,27 @@
       <c r="S66" s="1"/>
     </row>
     <row r="67" spans="1:19" ht="51" customHeight="1">
-      <c r="A67" s="15"/>
-      <c r="B67" s="15"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="15"/>
-      <c r="L67" s="15"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="15"/>
-      <c r="O67" s="15"/>
-      <c r="P67" s="15"/>
-      <c r="Q67" s="15"/>
-      <c r="R67" s="15"/>
-      <c r="S67" s="15"/>
-    </row>
-    <row r="68" spans="1:19" ht="30" customHeight="1">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="16"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+    </row>
+    <row r="68" spans="1:19" ht="51" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3570,12 +3356,12 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
-      <c r="J69" s="16"/>
-      <c r="K69" s="16"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
+      <c r="O69" s="16"/>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
@@ -3591,12 +3377,12 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
-      <c r="J70" s="16"/>
-      <c r="K70" s="16"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
+      <c r="O70" s="16"/>
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
@@ -3612,12 +3398,12 @@
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
+      <c r="O71" s="16"/>
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
@@ -3633,12 +3419,12 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="16"/>
-      <c r="K72" s="16"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
+      <c r="O72" s="16"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
@@ -3812,7 +3598,7 @@
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
     </row>
-    <row r="81" spans="1:19" ht="51" customHeight="1">
+    <row r="81" spans="1:19" ht="18.75" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3833,7 +3619,7 @@
       <c r="R81" s="1"/>
       <c r="S81" s="1"/>
     </row>
-    <row r="82" spans="1:19" ht="51" customHeight="1">
+    <row r="82" spans="1:19" ht="15.75" customHeight="1">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3854,7 +3640,7 @@
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
     </row>
-    <row r="83" spans="1:19" ht="51" customHeight="1">
+    <row r="83" spans="1:19" ht="15.75" customHeight="1">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3875,7 +3661,7 @@
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
     </row>
-    <row r="84" spans="1:19" ht="51" customHeight="1">
+    <row r="84" spans="1:19" ht="15.75" customHeight="1">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3896,7 +3682,7 @@
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
     </row>
-    <row r="85" spans="1:19" ht="51" customHeight="1">
+    <row r="85" spans="1:19" ht="15.75" customHeight="1">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3917,7 +3703,7 @@
       <c r="R85" s="1"/>
       <c r="S85" s="1"/>
     </row>
-    <row r="86" spans="1:19" ht="51" customHeight="1">
+    <row r="86" spans="1:19" ht="15.75" customHeight="1">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3938,7 +3724,7 @@
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
     </row>
-    <row r="87" spans="1:19" ht="18.75" customHeight="1">
+    <row r="87" spans="1:19" ht="15.75" customHeight="1">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -22838,132 +22624,6 @@
       <c r="R986" s="1"/>
       <c r="S986" s="1"/>
     </row>
-    <row r="987" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A987" s="1"/>
-      <c r="B987" s="1"/>
-      <c r="C987" s="1"/>
-      <c r="D987" s="1"/>
-      <c r="E987" s="1"/>
-      <c r="F987" s="1"/>
-      <c r="G987" s="1"/>
-      <c r="H987" s="1"/>
-      <c r="I987" s="1"/>
-      <c r="J987" s="1"/>
-      <c r="K987" s="1"/>
-      <c r="L987" s="1"/>
-      <c r="M987" s="1"/>
-      <c r="N987" s="1"/>
-      <c r="O987" s="16"/>
-      <c r="P987" s="1"/>
-      <c r="Q987" s="1"/>
-      <c r="R987" s="1"/>
-      <c r="S987" s="1"/>
-    </row>
-    <row r="988" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A988" s="1"/>
-      <c r="B988" s="1"/>
-      <c r="C988" s="1"/>
-      <c r="D988" s="1"/>
-      <c r="E988" s="1"/>
-      <c r="F988" s="1"/>
-      <c r="G988" s="1"/>
-      <c r="H988" s="1"/>
-      <c r="I988" s="1"/>
-      <c r="J988" s="1"/>
-      <c r="K988" s="1"/>
-      <c r="L988" s="1"/>
-      <c r="M988" s="1"/>
-      <c r="N988" s="1"/>
-      <c r="O988" s="16"/>
-      <c r="P988" s="1"/>
-      <c r="Q988" s="1"/>
-      <c r="R988" s="1"/>
-      <c r="S988" s="1"/>
-    </row>
-    <row r="989" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A989" s="1"/>
-      <c r="B989" s="1"/>
-      <c r="C989" s="1"/>
-      <c r="D989" s="1"/>
-      <c r="E989" s="1"/>
-      <c r="F989" s="1"/>
-      <c r="G989" s="1"/>
-      <c r="H989" s="1"/>
-      <c r="I989" s="1"/>
-      <c r="J989" s="1"/>
-      <c r="K989" s="1"/>
-      <c r="L989" s="1"/>
-      <c r="M989" s="1"/>
-      <c r="N989" s="1"/>
-      <c r="O989" s="16"/>
-      <c r="P989" s="1"/>
-      <c r="Q989" s="1"/>
-      <c r="R989" s="1"/>
-      <c r="S989" s="1"/>
-    </row>
-    <row r="990" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A990" s="1"/>
-      <c r="B990" s="1"/>
-      <c r="C990" s="1"/>
-      <c r="D990" s="1"/>
-      <c r="E990" s="1"/>
-      <c r="F990" s="1"/>
-      <c r="G990" s="1"/>
-      <c r="H990" s="1"/>
-      <c r="I990" s="1"/>
-      <c r="J990" s="1"/>
-      <c r="K990" s="1"/>
-      <c r="L990" s="1"/>
-      <c r="M990" s="1"/>
-      <c r="N990" s="1"/>
-      <c r="O990" s="16"/>
-      <c r="P990" s="1"/>
-      <c r="Q990" s="1"/>
-      <c r="R990" s="1"/>
-      <c r="S990" s="1"/>
-    </row>
-    <row r="991" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A991" s="1"/>
-      <c r="B991" s="1"/>
-      <c r="C991" s="1"/>
-      <c r="D991" s="1"/>
-      <c r="E991" s="1"/>
-      <c r="F991" s="1"/>
-      <c r="G991" s="1"/>
-      <c r="H991" s="1"/>
-      <c r="I991" s="1"/>
-      <c r="J991" s="1"/>
-      <c r="K991" s="1"/>
-      <c r="L991" s="1"/>
-      <c r="M991" s="1"/>
-      <c r="N991" s="1"/>
-      <c r="O991" s="16"/>
-      <c r="P991" s="1"/>
-      <c r="Q991" s="1"/>
-      <c r="R991" s="1"/>
-      <c r="S991" s="1"/>
-    </row>
-    <row r="992" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A992" s="1"/>
-      <c r="B992" s="1"/>
-      <c r="C992" s="1"/>
-      <c r="D992" s="1"/>
-      <c r="E992" s="1"/>
-      <c r="F992" s="1"/>
-      <c r="G992" s="1"/>
-      <c r="H992" s="1"/>
-      <c r="I992" s="1"/>
-      <c r="J992" s="1"/>
-      <c r="K992" s="1"/>
-      <c r="L992" s="1"/>
-      <c r="M992" s="1"/>
-      <c r="N992" s="1"/>
-      <c r="O992" s="16"/>
-      <c r="P992" s="1"/>
-      <c r="Q992" s="1"/>
-      <c r="R992" s="1"/>
-      <c r="S992" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.3" right="0.25" top="0.56999999999999995" bottom="0.75" header="0" footer="0"/>
   <pageSetup fitToHeight="0" orientation="landscape"/>
@@ -22972,15 +22632,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7E6DCC-2820-434A-9B82-123CB6A6D64E}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
@@ -23159,6 +22820,346 @@
         <v>60</v>
       </c>
     </row>
+    <row r="4" spans="1:19" ht="51" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14">
+        <v>18.33737</v>
+      </c>
+      <c r="F4" s="14">
+        <v>-65.082999999999998</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="51" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="4">
+        <v>18.330300000000001</v>
+      </c>
+      <c r="F5" s="4">
+        <v>-64.926400000000001</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="135">
+      <c r="A6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="4">
+        <v>41051</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4">
+        <v>18.257400000000001</v>
+      </c>
+      <c r="F6" s="4">
+        <v>-65.004000000000005</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="51" customHeight="1">
+      <c r="A7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4">
+        <v>17.9694</v>
+      </c>
+      <c r="F7" s="4">
+        <v>-67.044200000000004</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="135">
+      <c r="A8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="4">
+        <v>41051</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4">
+        <v>18.476099999999999</v>
+      </c>
+      <c r="F8" s="4">
+        <v>-65.156800000000004</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="51" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="14">
+        <v>18.355370000000001</v>
+      </c>
+      <c r="F9" s="14">
+        <v>-64.966930000000005</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>